<commit_message>
add requirement groups for sub-requirements
</commit_message>
<xml_diff>
--- a/lib/bulk_data_test_kit/requirements/hl7.fhir.uv.bulkdata_2.0.0_reqs.xlsx
+++ b/lib/bulk_data_test_kit/requirements/hl7.fhir.uv.bulkdata_2.0.0_reqs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/bulk-data-test-kit/lib/bulk_data_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86864A3B-30D3-0646-A1BF-65B926A16F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1866BA7-C595-F74B-AF2F-2056B784EB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1680" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="940" yWindow="1680" windowWidth="33080" windowHeight="18880" activeTab="3" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="494">
   <si>
     <r>
       <rPr>
@@ -2760,6 +2760,56 @@
     </r>
   </si>
   <si>
+    <t>A FHIR Bulk Data Client has the option of choosing from this list [of supported operations] to access necessary data based on use cases and other contextual requirements.</t>
+  </si>
+  <si>
+    <t>Depends on MAY params requirements for support of _typeFilter</t>
+  </si>
+  <si>
+    <t>hl7.fhir.uv.bulkdata_2.0.0@169-176</t>
+  </si>
+  <si>
+    <t>Actors*</t>
+  </si>
+  <si>
+    <t>reserved by addition in bulk STU 1</t>
+  </si>
+  <si>
+    <t>hl7.fhir.uv.smart-app-launch_2.0.0@30,228,231,240,241,243-262,265,266,285-289,296,297,305,306,310,311,316,326,335-342,344,372-374,376,377,380-386,389-394,438,439</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>System-level</t>
+  </si>
+  <si>
+    <t>Group-level</t>
+  </si>
+  <si>
+    <t>Patient-level, Group-level</t>
+  </si>
+  <si>
+    <t>Patient-level</t>
+  </si>
+  <si>
+    <t>- General = general requirements applicable to all systems
+- Security = security requirements. May not be included in when referenced if the referenced spec has its own security requirements
+- Export = requirements applicable to all systems regardless of which level of $export operations are supported
+- System-level = requirements applicable to systems implementing system-level $export
+- Group-level = requirements applicable to systems implementing group-level $export
+-Patient-level = requirements applicable to systems implementing patient-level $export</t>
+  </si>
+  <si>
+    <t>Groupings (Column P)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Metadata
 </t>
@@ -2966,26 +3016,29 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E.g., for  Da Vinci Payer Data Exchange (v2.0.0: STU2), Reference would be https://hl7.org/fhir/us/davinci-pdex/STU2/.</t>
+      <t xml:space="preserve">E.g., for  Da Vinci Payer Data Exchange (v2.0.0: STU2), Reference would be https://hl7.org/fhir/us/davinci-pdex/STU2/.
+ Additional metadata:
+</t>
     </r>
-  </si>
-  <si>
-    <t>A FHIR Bulk Data Client has the option of choosing from this list [of supported operations] to access necessary data based on use cases and other contextual requirements.</t>
-  </si>
-  <si>
-    <t>Depends on MAY params requirements for support of _typeFilter</t>
-  </si>
-  <si>
-    <t>hl7.fhir.uv.bulkdata_2.0.0@169-176</t>
-  </si>
-  <si>
-    <t>Actors*</t>
-  </si>
-  <si>
-    <t>reserved by addition in bulk STU 1</t>
-  </si>
-  <si>
-    <t>hl7.fhir.uv.smart-app-launch_2.0.0@30,228,231,240,241,243-262,265,266,285-289,296,297,305,306,310,311,316,326,335-342,344,372-374,376,377,380-386,389-394,438,439</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Groupings (Column P)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: definitions of the Groupings in Column P of the Requirements sheet.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3138,7 +3191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3202,6 +3255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -3463,7 +3522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3607,6 +3666,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4044,14 +4107,14 @@
       <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>477</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="36"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="68"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="39"/>
       <c r="C5" s="34"/>
     </row>
@@ -4063,17 +4126,17 @@
       <c r="C6" s="27"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="72"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="73"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="38"/>
     </row>
     <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
@@ -4098,11 +4161,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:AE318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="U5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F319" sqref="F319"/>
+      <selection pane="bottomRight" activeCell="R323" sqref="R323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4143,7 +4206,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
@@ -4242,7 +4305,9 @@
         <v>Server</v>
       </c>
       <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="R2" s="10" t="s">
+        <v>484</v>
+      </c>
       <c r="S2" s="16"/>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -4292,7 +4357,9 @@
         <v>Server</v>
       </c>
       <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
+      <c r="R3" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="S3" s="16"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -4335,6 +4402,9 @@
       <c r="P4" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>485</v>
       </c>
       <c r="V4" s="10" t="s">
         <v>38</v>
@@ -4364,7 +4434,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G5" s="7" t="b">
         <v>0</v>
@@ -4384,6 +4454,9 @@
       <c r="P5" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>485</v>
       </c>
       <c r="V5" s="16" t="s">
         <v>463</v>
@@ -4431,6 +4504,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R6" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="14"/>
       <c r="Z6" s="5"/>
@@ -4471,6 +4547,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R7" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="X7" s="5"/>
       <c r="Y7" s="14"/>
       <c r="Z7" s="5"/>
@@ -4511,6 +4590,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R8" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="X8" s="5"/>
       <c r="Y8" s="14"/>
       <c r="Z8" s="5"/>
@@ -4551,6 +4633,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R9" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="10" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -4587,6 +4672,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R10" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="11" spans="1:31" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
@@ -4623,6 +4711,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R11" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="12" spans="1:31" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
@@ -4659,6 +4750,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R12" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="13" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
@@ -4695,6 +4789,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R13" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="14" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
@@ -4731,6 +4828,9 @@
         <f>IF(ISNUMBER(SEARCH("server", C14)), "Server", IF(ISNUMBER(SEARCH("Server", C14)), "Server", IF(ISNUMBER(SEARCH("client", C14)), "Client", IF(ISNUMBER(SEARCH("Client", C14)), "Client", ""))))</f>
         <v>Server</v>
       </c>
+      <c r="R14" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="15" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -4767,6 +4867,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R15" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="16" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -4803,6 +4906,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R16" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="17" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -4839,6 +4945,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R17" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="18" spans="1:23" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -4881,6 +4990,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R18" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S18" s="16" t="s">
         <v>58</v>
       </c>
@@ -4923,6 +5035,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R19" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="W19" s="6" t="s">
         <v>61</v>
       </c>
@@ -4962,6 +5077,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R20" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="21" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -4998,6 +5116,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R21" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="22" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -5034,6 +5155,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R22" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="23" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -5070,6 +5194,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R23" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="24" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -5106,6 +5233,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R24" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="T24" s="16"/>
     </row>
     <row r="25" spans="1:23" ht="34" x14ac:dyDescent="0.2">
@@ -5143,6 +5273,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R25" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="26" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
@@ -5179,6 +5312,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R26" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="27" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
@@ -5254,6 +5390,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R28" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="29" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
@@ -5290,6 +5429,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R29" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="30" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
@@ -5326,6 +5468,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R30" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="31" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
@@ -5362,6 +5507,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R31" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="32" spans="1:23" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
@@ -5401,6 +5549,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R32" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S32" s="16" t="s">
         <v>80</v>
       </c>
@@ -5447,6 +5598,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R33" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="34" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
@@ -5486,6 +5640,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R34" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="35" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
@@ -5525,6 +5682,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R35" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="36" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
@@ -5564,6 +5724,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R36" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="37" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
@@ -5603,6 +5766,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R37" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="38" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
@@ -5642,6 +5808,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R38" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="39" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
@@ -5681,6 +5850,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R39" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="40" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
@@ -5717,6 +5889,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R40" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="41" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
@@ -5753,6 +5928,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R41" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="42" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
@@ -5789,6 +5967,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R42" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="43" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
@@ -5828,6 +6009,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R43" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="44" spans="1:20" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
@@ -5870,6 +6054,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R44" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S44" s="16" t="s">
         <v>80</v>
       </c>
@@ -5912,6 +6099,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R45" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="46" spans="1:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
@@ -5954,6 +6144,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R46" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S46" s="16" t="s">
         <v>80</v>
       </c>
@@ -5996,6 +6189,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R47" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="48" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
@@ -6032,6 +6228,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R48" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="49" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
@@ -6071,6 +6270,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R49" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S49" s="16" t="s">
         <v>80</v>
       </c>
@@ -6110,6 +6312,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R50" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="51" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
@@ -6146,6 +6351,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R51" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="52" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
@@ -6182,6 +6390,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R52" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="53" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
@@ -6218,6 +6429,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R53" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="54" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
@@ -6254,6 +6468,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R54" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="55" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
@@ -6293,6 +6510,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R55" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S55" s="16" t="s">
         <v>80</v>
       </c>
@@ -6335,6 +6555,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R56" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="57" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
@@ -6374,6 +6597,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R57" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="58" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
@@ -6413,6 +6639,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R58" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="59" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
@@ -6452,6 +6681,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R59" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="60" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
@@ -6488,6 +6720,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R60" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="61" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
@@ -6524,6 +6759,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R61" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="62" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
@@ -6563,6 +6801,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R62" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S62" s="16" t="s">
         <v>80</v>
       </c>
@@ -6605,6 +6846,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R63" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="64" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
@@ -6644,6 +6888,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R64" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="65" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
@@ -6683,6 +6930,9 @@
         <f t="shared" ref="P65:P128" si="2">IF(ISNUMBER(SEARCH("server", C65)), "Server", IF(ISNUMBER(SEARCH("Server", C65)), "Server", IF(ISNUMBER(SEARCH("client", C65)), "Client", IF(ISNUMBER(SEARCH("Client", C65)), "Client", ""))))</f>
         <v/>
       </c>
+      <c r="R65" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="66" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
@@ -6722,6 +6972,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R66" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="67" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
@@ -6761,6 +7014,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R67" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="68" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
@@ -6800,6 +7056,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R68" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="69" spans="1:19" ht="238" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
@@ -6839,6 +7098,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R69" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="70" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
@@ -6878,6 +7140,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R70" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="71" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
@@ -6917,6 +7182,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R71" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="72" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
@@ -6956,6 +7224,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R72" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="73" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
@@ -6995,6 +7266,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R73" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="74" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
@@ -7028,6 +7302,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R74" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="75" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
@@ -7064,6 +7341,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R75" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S75" s="16" t="s">
         <v>80</v>
       </c>
@@ -7106,6 +7386,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R76" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="77" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
@@ -7145,6 +7428,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R77" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="78" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
@@ -7184,6 +7470,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R78" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="79" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
@@ -7223,6 +7512,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R79" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="80" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
@@ -7262,6 +7554,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R80" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="81" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
@@ -7301,6 +7596,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R81" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="82" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
@@ -7340,6 +7638,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R82" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="83" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
@@ -7379,12 +7680,15 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R83" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="84" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>83</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B84" s="11" t="s">
         <v>104</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -7415,6 +7719,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R84" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="85" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
@@ -7454,6 +7761,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R85" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S85" s="16" t="s">
         <v>80</v>
       </c>
@@ -7496,6 +7806,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R86" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="87" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
@@ -7535,6 +7848,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R87" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="88" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
@@ -7574,6 +7890,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R88" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="89" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
@@ -7613,6 +7932,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R89" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="90" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
@@ -7652,6 +7974,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R90" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="91" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
@@ -7688,6 +8013,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R91" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="92" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
@@ -7727,6 +8055,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R92" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S92" s="16" t="s">
         <v>80</v>
       </c>
@@ -7769,6 +8100,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R93" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="94" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
@@ -7808,6 +8142,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R94" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="95" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
@@ -7847,6 +8184,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R95" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="96" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
@@ -7889,6 +8229,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R96" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S96" s="16" t="s">
         <v>80</v>
       </c>
@@ -7934,6 +8277,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R97" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="98" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
@@ -7973,6 +8319,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R98" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="99" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
@@ -8012,6 +8361,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R99" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="100" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
@@ -8051,6 +8403,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R100" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="101" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
@@ -8090,6 +8445,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R101" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="102" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
@@ -8126,6 +8484,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R102" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="103" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
@@ -8165,6 +8526,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R103" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S103" s="16" t="s">
         <v>80</v>
       </c>
@@ -8207,6 +8571,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R104" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="105" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
@@ -8237,7 +8604,7 @@
         <v>78</v>
       </c>
       <c r="L105" s="30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M105" s="9" t="str" cm="1">
         <f t="array" ref="M105">PAGE_NAME(B105)</f>
@@ -8255,6 +8622,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R105" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S105" s="16" t="s">
         <v>80</v>
       </c>
@@ -8297,6 +8667,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R106" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="107" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
@@ -8336,6 +8709,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R107" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="108" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
@@ -8372,6 +8748,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R108" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="109" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
@@ -8411,6 +8790,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R109" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="110" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
@@ -8451,6 +8833,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R110" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="111" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
@@ -8490,6 +8875,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R111" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="112" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
@@ -8529,6 +8917,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R112" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="113" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
@@ -8568,6 +8959,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R113" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="114" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
@@ -8607,6 +9001,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R114" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S114" s="16" t="s">
         <v>80</v>
       </c>
@@ -8640,7 +9037,7 @@
         <v>78</v>
       </c>
       <c r="L115" s="30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M115" s="9" t="str" cm="1">
         <f t="array" ref="M115">PAGE_NAME(B115)</f>
@@ -8658,6 +9055,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R115" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S115" s="16" t="s">
         <v>80</v>
       </c>
@@ -8697,6 +9097,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R116" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="W116" s="6" t="s">
         <v>61</v>
       </c>
@@ -8739,6 +9142,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R117" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S117" s="16" t="s">
         <v>80</v>
       </c>
@@ -8778,6 +9184,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R118" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="119" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
@@ -8817,6 +9226,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R119" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="120" spans="1:23" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
@@ -8859,6 +9271,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R120" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S120" s="16" t="s">
         <v>58</v>
       </c>
@@ -8904,6 +9319,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R121" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="122" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
@@ -8943,6 +9361,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R122" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="123" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
@@ -8982,6 +9403,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R123" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="124" spans="1:23" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
@@ -9024,6 +9448,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R124" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S124" s="16" t="s">
         <v>58</v>
       </c>
@@ -9072,6 +9499,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R125" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S125" s="16" t="s">
         <v>80</v>
       </c>
@@ -9120,6 +9550,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R126" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="127" spans="1:23" ht="242.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
@@ -9162,6 +9595,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R127" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S127" s="16" t="s">
         <v>80</v>
       </c>
@@ -9207,6 +9643,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R128" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="129" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
@@ -9246,6 +9685,9 @@
         <f t="shared" ref="P129:P194" si="4">IF(ISNUMBER(SEARCH("server", C129)), "Server", IF(ISNUMBER(SEARCH("Server", C129)), "Server", IF(ISNUMBER(SEARCH("client", C129)), "Client", IF(ISNUMBER(SEARCH("Client", C129)), "Client", ""))))</f>
         <v>Server</v>
       </c>
+      <c r="R129" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="130" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
@@ -9285,6 +9727,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R130" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="131" spans="1:23" ht="202.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
@@ -9327,6 +9772,9 @@
         <f t="shared" si="4"/>
         <v>Client</v>
       </c>
+      <c r="R131" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S131" s="16" t="s">
         <v>80</v>
       </c>
@@ -9372,6 +9820,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R132" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="133" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
@@ -9408,6 +9859,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R133" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="134" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
@@ -9444,6 +9898,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R134" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="135" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
@@ -9480,6 +9937,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R135" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="136" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
@@ -9515,6 +9975,9 @@
       <c r="P136" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Client</v>
+      </c>
+      <c r="R136" s="10" t="s">
+        <v>486</v>
       </c>
       <c r="W136" s="6" t="s">
         <v>61</v>
@@ -9559,6 +10022,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R137" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S137" s="10"/>
     </row>
     <row r="138" spans="1:23" ht="68" x14ac:dyDescent="0.2">
@@ -9599,6 +10065,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R138" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="139" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
@@ -9635,6 +10104,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R139" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="140" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
@@ -9674,6 +10146,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R140" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="141" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
@@ -9713,6 +10188,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R141" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="142" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
@@ -9752,6 +10230,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R142" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="143" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
@@ -9791,6 +10272,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R143" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="144" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
@@ -9830,6 +10314,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R144" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="145" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
@@ -9866,6 +10353,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R145" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="146" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
@@ -9902,6 +10392,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R146" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="147" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
@@ -9938,6 +10431,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R147" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="W147" s="13"/>
     </row>
     <row r="148" spans="1:23" ht="85" x14ac:dyDescent="0.2">
@@ -9975,6 +10471,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R148" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="149" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
@@ -10011,6 +10510,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R149" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="150" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
@@ -10047,6 +10549,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R150" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="151" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
@@ -10083,6 +10588,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R151" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="152" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
@@ -10119,6 +10627,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R152" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="153" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
@@ -10155,6 +10666,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R153" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="154" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
@@ -10191,6 +10705,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R154" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="155" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
@@ -10227,6 +10744,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R155" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="156" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
@@ -10263,6 +10783,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R156" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="157" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
@@ -10299,6 +10822,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R157" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="158" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
@@ -10335,6 +10861,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R158" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="159" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
@@ -10374,6 +10903,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R159" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="160" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
@@ -10410,8 +10942,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="161" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R160" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
         <v>160</v>
       </c>
@@ -10446,8 +10981,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="162" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R161" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
         <v>161</v>
       </c>
@@ -10482,8 +11020,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="163" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R162" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
         <v>162</v>
       </c>
@@ -10521,8 +11062,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="164" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R163" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
         <v>163</v>
       </c>
@@ -10557,8 +11101,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="165" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R164" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A165" s="7">
         <v>164</v>
       </c>
@@ -10593,8 +11140,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="166" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R165" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A166" s="7">
         <v>165</v>
       </c>
@@ -10629,8 +11179,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="167" spans="1:16" ht="136" x14ac:dyDescent="0.2">
+      <c r="R166" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" ht="136" x14ac:dyDescent="0.2">
       <c r="A167" s="7">
         <v>166</v>
       </c>
@@ -10665,8 +11218,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="168" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R167" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
         <v>167</v>
       </c>
@@ -10704,8 +11260,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="169" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R168" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
         <v>168</v>
       </c>
@@ -10722,7 +11281,7 @@
         <v>31</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G169" s="7" t="b">
         <v>0</v>
@@ -10743,8 +11302,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="170" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R169" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
         <v>169</v>
       </c>
@@ -10779,8 +11341,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="171" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R170" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
         <v>170</v>
       </c>
@@ -10815,8 +11380,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="172" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R171" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
         <v>171</v>
       </c>
@@ -10851,8 +11419,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="173" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R172" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A173" s="7">
         <v>172</v>
       </c>
@@ -10887,8 +11458,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="174" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R173" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
         <v>173</v>
       </c>
@@ -10926,8 +11500,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="175" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R174" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A175" s="7">
         <v>174</v>
       </c>
@@ -10962,8 +11539,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="176" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R175" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A176" s="7">
         <v>175</v>
       </c>
@@ -10998,8 +11578,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="177" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R176" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A177" s="7">
         <v>176</v>
       </c>
@@ -11034,8 +11617,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="178" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R177" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A178" s="7">
         <v>177</v>
       </c>
@@ -11073,8 +11659,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="179" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R178" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A179" s="7">
         <v>178</v>
       </c>
@@ -11109,8 +11698,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="180" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R179" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A180" s="7">
         <v>179</v>
       </c>
@@ -11145,8 +11737,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="181" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R180" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A181" s="7">
         <v>180</v>
       </c>
@@ -11181,8 +11776,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="182" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R181" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A182" s="7">
         <v>181</v>
       </c>
@@ -11220,8 +11818,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="183" spans="1:16" ht="153" x14ac:dyDescent="0.2">
+      <c r="R182" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" ht="153" x14ac:dyDescent="0.2">
       <c r="A183" s="7">
         <v>182</v>
       </c>
@@ -11259,8 +11860,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="184" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R183" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A184" s="7">
         <v>183</v>
       </c>
@@ -11298,8 +11902,11 @@
         <f t="shared" ref="P184:P186" si="7">IF(ISNUMBER(SEARCH("server", C184)), "Server", IF(ISNUMBER(SEARCH("Server", C184)), "Server", IF(ISNUMBER(SEARCH("client", C184)), "Client", IF(ISNUMBER(SEARCH("Client", C184)), "Client", ""))))</f>
         <v>Server</v>
       </c>
-    </row>
-    <row r="185" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R184" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A185" s="7">
         <v>184</v>
       </c>
@@ -11337,8 +11944,11 @@
         <f t="shared" si="7"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="186" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R185" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A186" s="7">
         <v>185</v>
       </c>
@@ -11376,8 +11986,11 @@
         <f t="shared" si="7"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="187" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R186" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A187" s="7">
         <v>186</v>
       </c>
@@ -11412,8 +12025,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="188" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R187" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A188" s="7">
         <v>187</v>
       </c>
@@ -11448,8 +12064,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="189" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R188" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A189" s="7">
         <v>188</v>
       </c>
@@ -11484,8 +12103,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="190" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R189" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A190" s="7">
         <v>189</v>
       </c>
@@ -11520,8 +12142,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="191" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R190" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
         <v>190</v>
       </c>
@@ -11556,8 +12181,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="192" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R191" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A192" s="7">
         <v>191</v>
       </c>
@@ -11592,6 +12220,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R192" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="193" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A193" s="7">
@@ -11628,6 +12259,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R193" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="194" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A194" s="7">
@@ -11667,6 +12301,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R194" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="195" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A195" s="7">
@@ -11703,6 +12340,9 @@
         <f t="shared" ref="P195:P258" si="8">IF(ISNUMBER(SEARCH("server", C195)), "Server", IF(ISNUMBER(SEARCH("Server", C195)), "Server", IF(ISNUMBER(SEARCH("client", C195)), "Client", IF(ISNUMBER(SEARCH("Client", C195)), "Client", ""))))</f>
         <v/>
       </c>
+      <c r="R195" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="196" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A196" s="7">
@@ -11742,6 +12382,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R196" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="197" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A197" s="7">
@@ -11778,6 +12421,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R197" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="198" spans="1:23" ht="136" x14ac:dyDescent="0.2">
       <c r="A198" s="7">
@@ -11817,6 +12463,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R198" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="199" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A199" s="7">
@@ -11853,6 +12502,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R199" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="200" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A200" s="7">
@@ -11889,6 +12541,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R200" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="201" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A201" s="7">
@@ -11931,6 +12586,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R201" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S201" s="16" t="s">
         <v>58</v>
       </c>
@@ -11982,6 +12640,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R202" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S202" s="16" t="s">
         <v>80</v>
       </c>
@@ -12024,6 +12685,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R203" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="204" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A204" s="7">
@@ -12060,6 +12724,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R204" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="205" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A205" s="7">
@@ -12096,6 +12763,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R205" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="206" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A206" s="7">
@@ -12132,6 +12802,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R206" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="207" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A207" s="7">
@@ -12168,6 +12841,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R207" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="208" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A208" s="7">
@@ -12204,6 +12880,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R208" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="209" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A209" s="7">
@@ -12240,6 +12919,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R209" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="210" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A210" s="7">
@@ -12276,6 +12958,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R210" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="211" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A211" s="7">
@@ -12312,6 +12997,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R211" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="212" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A212" s="7">
@@ -12351,6 +13039,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R212" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="213" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A213" s="7">
@@ -12390,6 +13081,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R213" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="214" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A214" s="7">
@@ -12429,6 +13123,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R214" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="215" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A215" s="7">
@@ -12468,6 +13165,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R215" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="216" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A216" s="7">
@@ -12507,6 +13207,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R216" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="217" spans="1:22" ht="85" x14ac:dyDescent="0.2">
       <c r="A217" s="7">
@@ -12546,6 +13249,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R217" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="218" spans="1:22" ht="85" x14ac:dyDescent="0.2">
       <c r="A218" s="7">
@@ -12582,6 +13288,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R218" s="10" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="219" spans="1:22" ht="238" x14ac:dyDescent="0.2">
       <c r="A219" s="7">
@@ -12600,7 +13309,7 @@
         <v>31</v>
       </c>
       <c r="F219" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G219" s="7" t="b">
         <v>0</v>
@@ -12621,6 +13330,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R219" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="V219" s="16" t="s">
         <v>463</v>
       </c>
@@ -12696,6 +13408,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R221" s="10" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="222" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A222" s="7">
@@ -12705,7 +13420,7 @@
         <v>366</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D222" s="7" t="s">
         <v>37</v>
@@ -12735,6 +13450,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R222" s="10" t="s">
+        <v>484</v>
+      </c>
       <c r="S222" s="16" t="s">
         <v>80</v>
       </c>
@@ -12814,6 +13532,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R224" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="225" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A225" s="7">
@@ -12854,6 +13575,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R225" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="226" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A226" s="7">
@@ -12894,6 +13618,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R226" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="227" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A227" s="7">
@@ -12930,6 +13657,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R227" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="228" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A228" s="7">
@@ -12966,6 +13696,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R228" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="229" spans="1:22" ht="85" x14ac:dyDescent="0.2">
       <c r="A229" s="7">
@@ -13002,6 +13735,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R229" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="230" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A230" s="7">
@@ -13038,6 +13774,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R230" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="231" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A231" s="7">
@@ -13113,6 +13852,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R232" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="233" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A233" s="7">
@@ -13149,6 +13891,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R233" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="234" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A234" s="7">
@@ -13221,6 +13966,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R235" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="236" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A236" s="7">
@@ -13257,6 +14005,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R236" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="237" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A237" s="7">
@@ -13329,6 +14080,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R238" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="239" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A239" s="7">
@@ -13365,6 +14119,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R239" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="240" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A240" s="7">
@@ -13437,6 +14194,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R241" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="242" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="7">
@@ -13473,6 +14233,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R242" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="243" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A243" s="7">
@@ -13545,6 +14308,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R244" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="245" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A245" s="7">
@@ -13581,6 +14347,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R245" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="246" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A246" s="7">
@@ -13653,6 +14422,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R247" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="248" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A248" s="7">
@@ -13689,6 +14461,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R248" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="249" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A249" s="7">
@@ -13761,6 +14536,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R250" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="251" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A251" s="7">
@@ -13797,6 +14575,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R251" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="252" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A252" s="7">
@@ -13833,6 +14614,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R252" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="253" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A253" s="7">
@@ -13872,6 +14656,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R253" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S253" s="16" t="s">
         <v>80</v>
       </c>
@@ -13947,6 +14734,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R255" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="256" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A256" s="7">
@@ -13986,6 +14776,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R256" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S256" s="16" t="s">
         <v>80</v>
       </c>
@@ -14061,6 +14854,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R258" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="259" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" s="7">
@@ -14100,6 +14896,9 @@
         <f t="shared" ref="P259:P272" si="10">IF(ISNUMBER(SEARCH("server", C259)), "Server", IF(ISNUMBER(SEARCH("Server", C259)), "Server", IF(ISNUMBER(SEARCH("client", C259)), "Client", IF(ISNUMBER(SEARCH("Client", C259)), "Client", ""))))</f>
         <v>Client</v>
       </c>
+      <c r="R259" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S259" s="16" t="s">
         <v>80</v>
       </c>
@@ -14175,6 +14974,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R261" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="262" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A262" s="7">
@@ -14214,6 +15016,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R262" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S262" s="16" t="s">
         <v>80</v>
       </c>
@@ -14289,6 +15094,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R264" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="265" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A265" s="7">
@@ -14328,6 +15136,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R265" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S265" s="16" t="s">
         <v>80</v>
       </c>
@@ -14403,6 +15214,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R267" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="268" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A268" s="7">
@@ -14442,6 +15256,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R268" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S268" s="16" t="s">
         <v>80</v>
       </c>
@@ -14517,6 +15334,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R270" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="271" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A271" s="7">
@@ -14556,6 +15376,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R271" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S271" s="16" t="s">
         <v>80</v>
       </c>
@@ -14596,7 +15419,7 @@
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A273" s="7">
         <v>272</v>
       </c>
@@ -14631,8 +15454,11 @@
         <f>IF(ISNUMBER(SEARCH("server", C273)), "Server", IF(ISNUMBER(SEARCH("Server", C273)), "Server", IF(ISNUMBER(SEARCH("client", C273)), "Client", IF(ISNUMBER(SEARCH("Client", C273)), "Client", ""))))</f>
         <v>Server</v>
       </c>
-    </row>
-    <row r="274" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R273" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="274" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A274" s="7">
         <v>273</v>
       </c>
@@ -14667,8 +15493,11 @@
         <f t="shared" ref="P274:P298" si="12">IF(ISNUMBER(SEARCH("server", C274)), "Server", IF(ISNUMBER(SEARCH("Server", C274)), "Server", IF(ISNUMBER(SEARCH("client", C274)), "Client", IF(ISNUMBER(SEARCH("Client", C274)), "Client", ""))))</f>
         <v/>
       </c>
-    </row>
-    <row r="275" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R274" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="275" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A275" s="7">
         <v>274</v>
       </c>
@@ -14703,8 +15532,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="276" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R275" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="276" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A276" s="7">
         <v>275</v>
       </c>
@@ -14739,8 +15571,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="277" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R276" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="277" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A277" s="7">
         <v>276</v>
       </c>
@@ -14776,7 +15611,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A278" s="7">
         <v>277</v>
       </c>
@@ -14811,8 +15646,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="279" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R278" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="279" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A279" s="7">
         <v>278</v>
       </c>
@@ -14847,8 +15685,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="280" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R279" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="280" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A280" s="7">
         <v>279</v>
       </c>
@@ -14884,7 +15725,7 @@
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A281" s="7">
         <v>280</v>
       </c>
@@ -14919,8 +15760,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="282" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R281" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="282" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A282" s="7">
         <v>281</v>
       </c>
@@ -14955,8 +15799,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="283" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R282" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="283" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A283" s="7">
         <v>282</v>
       </c>
@@ -14992,7 +15839,7 @@
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A284" s="7">
         <v>283</v>
       </c>
@@ -15027,8 +15874,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="285" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R284" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="285" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A285" s="7">
         <v>284</v>
       </c>
@@ -15063,8 +15913,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="286" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R285" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="286" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A286" s="7">
         <v>285</v>
       </c>
@@ -15100,7 +15953,7 @@
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A287" s="7">
         <v>286</v>
       </c>
@@ -15135,8 +15988,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="288" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R287" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="288" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A288" s="7">
         <v>287</v>
       </c>
@@ -15171,6 +16027,9 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
+      <c r="R288" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="289" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A289" s="7">
@@ -15243,6 +16102,9 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
+      <c r="R290" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="291" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A291" s="7">
@@ -15279,6 +16141,9 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
+      <c r="R291" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="292" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A292" s="7">
@@ -15351,6 +16216,9 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
+      <c r="R293" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="294" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A294" s="7">
@@ -15386,6 +16254,9 @@
       <c r="P294" s="10" t="str">
         <f t="shared" si="12"/>
         <v>Client</v>
+      </c>
+      <c r="R294" s="10" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="295" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -15466,7 +16337,9 @@
         <v>Server</v>
       </c>
       <c r="Q296" s="10"/>
-      <c r="R296" s="10"/>
+      <c r="R296" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="S296" s="16"/>
       <c r="T296" s="10"/>
       <c r="U296" s="10"/>
@@ -15475,7 +16348,7 @@
       </c>
       <c r="Y296" s="14"/>
     </row>
-    <row r="297" spans="1:31" s="58" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:31" s="58" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A297" s="7">
         <v>296</v>
       </c>
@@ -15517,7 +16390,9 @@
         <v/>
       </c>
       <c r="Q297" s="57"/>
-      <c r="R297" s="57"/>
+      <c r="R297" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="S297" s="54"/>
       <c r="T297" s="57"/>
       <c r="U297" s="57"/>
@@ -15566,7 +16441,9 @@
         <v>Server</v>
       </c>
       <c r="Q298" s="50"/>
-      <c r="R298" s="50"/>
+      <c r="R298" s="10" t="s">
+        <v>490</v>
+      </c>
       <c r="S298" s="47"/>
       <c r="T298" s="50"/>
       <c r="U298" s="50"/>
@@ -15588,6 +16465,9 @@
       <c r="E299" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R299" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="300" spans="1:31" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="7">
@@ -15605,6 +16485,9 @@
       <c r="E300" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R300" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="301" spans="1:31" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="7">
@@ -15622,6 +16505,9 @@
       <c r="E301" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R301" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="302" spans="1:31" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="7">
@@ -15639,6 +16525,9 @@
       <c r="E302" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R302" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="303" spans="1:31" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="7">
@@ -15656,6 +16545,9 @@
       <c r="E303" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R303" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="304" spans="1:31" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="7">
@@ -15673,6 +16565,9 @@
       <c r="E304" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R304" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="305" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="7">
@@ -15690,6 +16585,9 @@
       <c r="E305" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R305" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="306" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="7">
@@ -15707,6 +16605,9 @@
       <c r="E306" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R306" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="307" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="7">
@@ -15724,6 +16625,9 @@
       <c r="E307" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R307" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="308" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="7">
@@ -15741,6 +16645,9 @@
       <c r="E308" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R308" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="309" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="7">
@@ -15758,6 +16665,9 @@
       <c r="E309" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R309" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="310" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="7">
@@ -15775,6 +16685,9 @@
       <c r="E310" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R310" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="311" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="7">
@@ -15792,6 +16705,9 @@
       <c r="E311" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R311" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="312" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="45">
@@ -15801,7 +16717,7 @@
         <v>71</v>
       </c>
       <c r="V312" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="313" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15812,7 +16728,7 @@
         <v>71</v>
       </c>
       <c r="V313" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="314" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15823,7 +16739,7 @@
         <v>71</v>
       </c>
       <c r="V314" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="315" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15834,7 +16750,7 @@
         <v>71</v>
       </c>
       <c r="V315" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="316" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15845,7 +16761,7 @@
         <v>71</v>
       </c>
       <c r="V316" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="317" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15856,7 +16772,7 @@
         <v>71</v>
       </c>
       <c r="V317" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="318" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15867,7 +16783,7 @@
         <v>71</v>
       </c>
       <c r="V318" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -15905,6 +16821,7 @@
     <hyperlink ref="B149" r:id="rId29" location="response---complete-status" xr:uid="{B0720E1E-4816-F842-82C8-C111E8C22B58}"/>
     <hyperlink ref="B229" r:id="rId30" location="bulkdataigcapabilitystatement" xr:uid="{4CF2CCA0-FA45-274E-B515-93FFD2130283}"/>
     <hyperlink ref="B228" r:id="rId31" location="bulkdataigcapabilitystatement" xr:uid="{5D27A2D1-DFBB-104F-ABC7-76F2A9211160}"/>
+    <hyperlink ref="B84" r:id="rId32" location="query-parameters" xr:uid="{32E0F273-4A07-D44B-AC1C-0A5D007653DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -15952,27 +16869,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="56.5" style="19" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="84.6640625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
-        <v>478</v>
-      </c>
-      <c r="B1" s="72"/>
+      <c r="A1" s="74" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -16051,6 +16968,14 @@
       </c>
       <c r="B13" s="19" t="s">
         <v>446</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Requirements groupings for sub-requirement calculation (#55)
* typo fix

* add requirement groups for sub-requirements
</commit_message>
<xml_diff>
--- a/lib/bulk_data_test_kit/requirements/hl7.fhir.uv.bulkdata_2.0.0_reqs.xlsx
+++ b/lib/bulk_data_test_kit/requirements/hl7.fhir.uv.bulkdata_2.0.0_reqs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/bulk-data-test-kit/lib/bulk_data_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86864A3B-30D3-0646-A1BF-65B926A16F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1866BA7-C595-F74B-AF2F-2056B784EB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1680" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="940" yWindow="1680" windowWidth="33080" windowHeight="18880" activeTab="3" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="494">
   <si>
     <r>
       <rPr>
@@ -2760,6 +2760,56 @@
     </r>
   </si>
   <si>
+    <t>A FHIR Bulk Data Client has the option of choosing from this list [of supported operations] to access necessary data based on use cases and other contextual requirements.</t>
+  </si>
+  <si>
+    <t>Depends on MAY params requirements for support of _typeFilter</t>
+  </si>
+  <si>
+    <t>hl7.fhir.uv.bulkdata_2.0.0@169-176</t>
+  </si>
+  <si>
+    <t>Actors*</t>
+  </si>
+  <si>
+    <t>reserved by addition in bulk STU 1</t>
+  </si>
+  <si>
+    <t>hl7.fhir.uv.smart-app-launch_2.0.0@30,228,231,240,241,243-262,265,266,285-289,296,297,305,306,310,311,316,326,335-342,344,372-374,376,377,380-386,389-394,438,439</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>System-level</t>
+  </si>
+  <si>
+    <t>Group-level</t>
+  </si>
+  <si>
+    <t>Patient-level, Group-level</t>
+  </si>
+  <si>
+    <t>Patient-level</t>
+  </si>
+  <si>
+    <t>- General = general requirements applicable to all systems
+- Security = security requirements. May not be included in when referenced if the referenced spec has its own security requirements
+- Export = requirements applicable to all systems regardless of which level of $export operations are supported
+- System-level = requirements applicable to systems implementing system-level $export
+- Group-level = requirements applicable to systems implementing group-level $export
+-Patient-level = requirements applicable to systems implementing patient-level $export</t>
+  </si>
+  <si>
+    <t>Groupings (Column P)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Metadata
 </t>
@@ -2966,26 +3016,29 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E.g., for  Da Vinci Payer Data Exchange (v2.0.0: STU2), Reference would be https://hl7.org/fhir/us/davinci-pdex/STU2/.</t>
+      <t xml:space="preserve">E.g., for  Da Vinci Payer Data Exchange (v2.0.0: STU2), Reference would be https://hl7.org/fhir/us/davinci-pdex/STU2/.
+ Additional metadata:
+</t>
     </r>
-  </si>
-  <si>
-    <t>A FHIR Bulk Data Client has the option of choosing from this list [of supported operations] to access necessary data based on use cases and other contextual requirements.</t>
-  </si>
-  <si>
-    <t>Depends on MAY params requirements for support of _typeFilter</t>
-  </si>
-  <si>
-    <t>hl7.fhir.uv.bulkdata_2.0.0@169-176</t>
-  </si>
-  <si>
-    <t>Actors*</t>
-  </si>
-  <si>
-    <t>reserved by addition in bulk STU 1</t>
-  </si>
-  <si>
-    <t>hl7.fhir.uv.smart-app-launch_2.0.0@30,228,231,240,241,243-262,265,266,285-289,296,297,305,306,310,311,316,326,335-342,344,372-374,376,377,380-386,389-394,438,439</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Groupings (Column P)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: definitions of the Groupings in Column P of the Requirements sheet.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3138,7 +3191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3202,6 +3255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -3463,7 +3522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3607,6 +3666,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4044,14 +4107,14 @@
       <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>477</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="36"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="68"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="39"/>
       <c r="C5" s="34"/>
     </row>
@@ -4063,17 +4126,17 @@
       <c r="C6" s="27"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="72"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="73"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="38"/>
     </row>
     <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
@@ -4098,11 +4161,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:AE318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="U5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F319" sqref="F319"/>
+      <selection pane="bottomRight" activeCell="R323" sqref="R323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4143,7 +4206,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
@@ -4242,7 +4305,9 @@
         <v>Server</v>
       </c>
       <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="R2" s="10" t="s">
+        <v>484</v>
+      </c>
       <c r="S2" s="16"/>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -4292,7 +4357,9 @@
         <v>Server</v>
       </c>
       <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
+      <c r="R3" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="S3" s="16"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -4335,6 +4402,9 @@
       <c r="P4" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>485</v>
       </c>
       <c r="V4" s="10" t="s">
         <v>38</v>
@@ -4364,7 +4434,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G5" s="7" t="b">
         <v>0</v>
@@ -4384,6 +4454,9 @@
       <c r="P5" s="10" t="str">
         <f t="shared" si="0"/>
         <v/>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>485</v>
       </c>
       <c r="V5" s="16" t="s">
         <v>463</v>
@@ -4431,6 +4504,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R6" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="X6" s="5"/>
       <c r="Y6" s="14"/>
       <c r="Z6" s="5"/>
@@ -4471,6 +4547,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R7" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="X7" s="5"/>
       <c r="Y7" s="14"/>
       <c r="Z7" s="5"/>
@@ -4511,6 +4590,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R8" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="X8" s="5"/>
       <c r="Y8" s="14"/>
       <c r="Z8" s="5"/>
@@ -4551,6 +4633,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R9" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="10" spans="1:31" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
@@ -4587,6 +4672,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R10" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="11" spans="1:31" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
@@ -4623,6 +4711,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R11" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="12" spans="1:31" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
@@ -4659,6 +4750,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R12" s="10" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="13" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
@@ -4695,6 +4789,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R13" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="14" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
@@ -4731,6 +4828,9 @@
         <f>IF(ISNUMBER(SEARCH("server", C14)), "Server", IF(ISNUMBER(SEARCH("Server", C14)), "Server", IF(ISNUMBER(SEARCH("client", C14)), "Client", IF(ISNUMBER(SEARCH("Client", C14)), "Client", ""))))</f>
         <v>Server</v>
       </c>
+      <c r="R14" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="15" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
@@ -4767,6 +4867,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R15" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="16" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
@@ -4803,6 +4906,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R16" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="17" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -4839,6 +4945,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R17" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="18" spans="1:23" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
@@ -4881,6 +4990,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R18" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S18" s="16" t="s">
         <v>58</v>
       </c>
@@ -4923,6 +5035,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R19" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="W19" s="6" t="s">
         <v>61</v>
       </c>
@@ -4962,6 +5077,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R20" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="21" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
@@ -4998,6 +5116,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R21" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="22" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
@@ -5034,6 +5155,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R22" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="23" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
@@ -5070,6 +5194,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R23" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="24" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
@@ -5106,6 +5233,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R24" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="T24" s="16"/>
     </row>
     <row r="25" spans="1:23" ht="34" x14ac:dyDescent="0.2">
@@ -5143,6 +5273,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R25" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="26" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
@@ -5179,6 +5312,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R26" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="27" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
@@ -5254,6 +5390,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R28" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="29" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
@@ -5290,6 +5429,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R29" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="30" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
@@ -5326,6 +5468,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R30" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="31" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
@@ -5362,6 +5507,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R31" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="32" spans="1:23" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
@@ -5401,6 +5549,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R32" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S32" s="16" t="s">
         <v>80</v>
       </c>
@@ -5447,6 +5598,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R33" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="34" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
@@ -5486,6 +5640,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R34" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="35" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
@@ -5525,6 +5682,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R35" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="36" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
@@ -5564,6 +5724,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R36" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="37" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
@@ -5603,6 +5766,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R37" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="38" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
@@ -5642,6 +5808,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R38" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="39" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
@@ -5681,6 +5850,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R39" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="40" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
@@ -5717,6 +5889,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R40" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="41" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
@@ -5753,6 +5928,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R41" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="42" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
@@ -5789,6 +5967,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R42" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="43" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
@@ -5828,6 +6009,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R43" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="44" spans="1:20" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
@@ -5870,6 +6054,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R44" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S44" s="16" t="s">
         <v>80</v>
       </c>
@@ -5912,6 +6099,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R45" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="46" spans="1:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
@@ -5954,6 +6144,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R46" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S46" s="16" t="s">
         <v>80</v>
       </c>
@@ -5996,6 +6189,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R47" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="48" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
@@ -6032,6 +6228,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R48" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="49" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
@@ -6071,6 +6270,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R49" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S49" s="16" t="s">
         <v>80</v>
       </c>
@@ -6110,6 +6312,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R50" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="51" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
@@ -6146,6 +6351,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R51" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="52" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
@@ -6182,6 +6390,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R52" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="53" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
@@ -6218,6 +6429,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R53" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="54" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
@@ -6254,6 +6468,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R54" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="55" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
@@ -6293,6 +6510,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R55" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S55" s="16" t="s">
         <v>80</v>
       </c>
@@ -6335,6 +6555,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R56" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="57" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
@@ -6374,6 +6597,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R57" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="58" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
@@ -6413,6 +6639,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R58" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="59" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
@@ -6452,6 +6681,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R59" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="60" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
@@ -6488,6 +6720,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R60" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="61" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
@@ -6524,6 +6759,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R61" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="62" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
@@ -6563,6 +6801,9 @@
         <f t="shared" si="0"/>
         <v>Client</v>
       </c>
+      <c r="R62" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S62" s="16" t="s">
         <v>80</v>
       </c>
@@ -6605,6 +6846,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="R63" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="64" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
@@ -6644,6 +6888,9 @@
         <f t="shared" si="0"/>
         <v>Server</v>
       </c>
+      <c r="R64" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="65" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
@@ -6683,6 +6930,9 @@
         <f t="shared" ref="P65:P128" si="2">IF(ISNUMBER(SEARCH("server", C65)), "Server", IF(ISNUMBER(SEARCH("Server", C65)), "Server", IF(ISNUMBER(SEARCH("client", C65)), "Client", IF(ISNUMBER(SEARCH("Client", C65)), "Client", ""))))</f>
         <v/>
       </c>
+      <c r="R65" s="67" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="66" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
@@ -6722,6 +6972,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R66" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="67" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
@@ -6761,6 +7014,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R67" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="68" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
@@ -6800,6 +7056,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R68" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="69" spans="1:19" ht="238" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
@@ -6839,6 +7098,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R69" s="67" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="70" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
@@ -6878,6 +7140,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R70" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="71" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
@@ -6917,6 +7182,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R71" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="72" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
@@ -6956,6 +7224,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R72" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="73" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
@@ -6995,6 +7266,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R73" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="74" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
@@ -7028,6 +7302,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R74" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="75" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
@@ -7064,6 +7341,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R75" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S75" s="16" t="s">
         <v>80</v>
       </c>
@@ -7106,6 +7386,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R76" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="77" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
@@ -7145,6 +7428,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R77" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="78" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
@@ -7184,6 +7470,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R78" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="79" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
@@ -7223,6 +7512,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R79" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="80" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
@@ -7262,6 +7554,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R80" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="81" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
@@ -7301,6 +7596,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R81" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="82" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
@@ -7340,6 +7638,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R82" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="83" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
@@ -7379,12 +7680,15 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R83" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="84" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>83</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B84" s="11" t="s">
         <v>104</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -7415,6 +7719,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R84" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="85" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
@@ -7454,6 +7761,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R85" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S85" s="16" t="s">
         <v>80</v>
       </c>
@@ -7496,6 +7806,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R86" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="87" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
@@ -7535,6 +7848,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R87" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="88" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
@@ -7574,6 +7890,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R88" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="89" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
@@ -7613,6 +7932,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R89" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="90" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
@@ -7652,6 +7974,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R90" s="10" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="91" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
@@ -7688,6 +8013,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R91" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="92" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
@@ -7727,6 +8055,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R92" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S92" s="16" t="s">
         <v>80</v>
       </c>
@@ -7769,6 +8100,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R93" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="94" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
@@ -7808,6 +8142,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R94" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="95" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
@@ -7847,6 +8184,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R95" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="96" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
@@ -7889,6 +8229,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R96" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S96" s="16" t="s">
         <v>80</v>
       </c>
@@ -7934,6 +8277,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R97" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="98" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
@@ -7973,6 +8319,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R98" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="99" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
@@ -8012,6 +8361,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R99" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="100" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
@@ -8051,6 +8403,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R100" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="101" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
@@ -8090,6 +8445,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R101" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="102" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
@@ -8126,6 +8484,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R102" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="103" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
@@ -8165,6 +8526,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R103" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S103" s="16" t="s">
         <v>80</v>
       </c>
@@ -8207,6 +8571,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R104" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="105" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
@@ -8237,7 +8604,7 @@
         <v>78</v>
       </c>
       <c r="L105" s="30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M105" s="9" t="str" cm="1">
         <f t="array" ref="M105">PAGE_NAME(B105)</f>
@@ -8255,6 +8622,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R105" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S105" s="16" t="s">
         <v>80</v>
       </c>
@@ -8297,6 +8667,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R106" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="107" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
@@ -8336,6 +8709,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R107" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="108" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
@@ -8372,6 +8748,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R108" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="109" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
@@ -8411,6 +8790,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R109" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="110" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
@@ -8451,6 +8833,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R110" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="111" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
@@ -8490,6 +8875,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R111" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="112" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
@@ -8529,6 +8917,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R112" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="113" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
@@ -8568,6 +8959,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R113" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="114" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
@@ -8607,6 +9001,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R114" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S114" s="16" t="s">
         <v>80</v>
       </c>
@@ -8640,7 +9037,7 @@
         <v>78</v>
       </c>
       <c r="L115" s="30" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M115" s="9" t="str" cm="1">
         <f t="array" ref="M115">PAGE_NAME(B115)</f>
@@ -8658,6 +9055,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="R115" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S115" s="16" t="s">
         <v>80</v>
       </c>
@@ -8697,6 +9097,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R116" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="W116" s="6" t="s">
         <v>61</v>
       </c>
@@ -8739,6 +9142,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R117" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S117" s="16" t="s">
         <v>80</v>
       </c>
@@ -8778,6 +9184,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R118" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="119" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
@@ -8817,6 +9226,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R119" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="120" spans="1:23" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
@@ -8859,6 +9271,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R120" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S120" s="16" t="s">
         <v>58</v>
       </c>
@@ -8904,6 +9319,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R121" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="122" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
@@ -8943,6 +9361,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R122" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="123" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
@@ -8982,6 +9403,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R123" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="124" spans="1:23" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
@@ -9024,6 +9448,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R124" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S124" s="16" t="s">
         <v>58</v>
       </c>
@@ -9072,6 +9499,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R125" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S125" s="16" t="s">
         <v>80</v>
       </c>
@@ -9120,6 +9550,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R126" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="127" spans="1:23" ht="242.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
@@ -9162,6 +9595,9 @@
         <f t="shared" si="2"/>
         <v>Client</v>
       </c>
+      <c r="R127" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S127" s="16" t="s">
         <v>80</v>
       </c>
@@ -9207,6 +9643,9 @@
         <f t="shared" si="2"/>
         <v>Server</v>
       </c>
+      <c r="R128" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="129" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
@@ -9246,6 +9685,9 @@
         <f t="shared" ref="P129:P194" si="4">IF(ISNUMBER(SEARCH("server", C129)), "Server", IF(ISNUMBER(SEARCH("Server", C129)), "Server", IF(ISNUMBER(SEARCH("client", C129)), "Client", IF(ISNUMBER(SEARCH("Client", C129)), "Client", ""))))</f>
         <v>Server</v>
       </c>
+      <c r="R129" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="130" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
@@ -9285,6 +9727,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R130" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="131" spans="1:23" ht="202.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
@@ -9327,6 +9772,9 @@
         <f t="shared" si="4"/>
         <v>Client</v>
       </c>
+      <c r="R131" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S131" s="16" t="s">
         <v>80</v>
       </c>
@@ -9372,6 +9820,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R132" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="133" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
@@ -9408,6 +9859,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R133" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="134" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
@@ -9444,6 +9898,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R134" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="135" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
@@ -9480,6 +9937,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R135" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="136" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
@@ -9515,6 +9975,9 @@
       <c r="P136" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Client</v>
+      </c>
+      <c r="R136" s="10" t="s">
+        <v>486</v>
       </c>
       <c r="W136" s="6" t="s">
         <v>61</v>
@@ -9559,6 +10022,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R137" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S137" s="10"/>
     </row>
     <row r="138" spans="1:23" ht="68" x14ac:dyDescent="0.2">
@@ -9599,6 +10065,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R138" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="139" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
@@ -9635,6 +10104,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R139" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="140" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
@@ -9674,6 +10146,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R140" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="141" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
@@ -9713,6 +10188,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R141" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="142" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
@@ -9752,6 +10230,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R142" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="143" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
@@ -9791,6 +10272,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R143" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="144" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
@@ -9830,6 +10314,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R144" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="145" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
@@ -9866,6 +10353,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R145" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="146" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
@@ -9902,6 +10392,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R146" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="147" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
@@ -9938,6 +10431,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R147" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="W147" s="13"/>
     </row>
     <row r="148" spans="1:23" ht="85" x14ac:dyDescent="0.2">
@@ -9975,6 +10471,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R148" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="149" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
@@ -10011,6 +10510,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R149" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="150" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
@@ -10047,6 +10549,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R150" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="151" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
@@ -10083,6 +10588,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R151" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="152" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
@@ -10119,6 +10627,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R152" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="153" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
@@ -10155,6 +10666,9 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
+      <c r="R153" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="154" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
@@ -10191,6 +10705,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R154" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="155" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
@@ -10227,6 +10744,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R155" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="156" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
@@ -10263,6 +10783,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R156" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="157" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
@@ -10299,6 +10822,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R157" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="158" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
@@ -10335,6 +10861,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R158" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="159" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
@@ -10374,6 +10903,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R159" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="160" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
@@ -10410,8 +10942,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="161" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R160" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
         <v>160</v>
       </c>
@@ -10446,8 +10981,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="162" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R161" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
         <v>161</v>
       </c>
@@ -10482,8 +11020,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="163" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R162" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
         <v>162</v>
       </c>
@@ -10521,8 +11062,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="164" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R163" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
         <v>163</v>
       </c>
@@ -10557,8 +11101,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="165" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R164" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A165" s="7">
         <v>164</v>
       </c>
@@ -10593,8 +11140,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="166" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R165" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A166" s="7">
         <v>165</v>
       </c>
@@ -10629,8 +11179,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="167" spans="1:16" ht="136" x14ac:dyDescent="0.2">
+      <c r="R166" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" ht="136" x14ac:dyDescent="0.2">
       <c r="A167" s="7">
         <v>166</v>
       </c>
@@ -10665,8 +11218,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="168" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R167" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
         <v>167</v>
       </c>
@@ -10704,8 +11260,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="169" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R168" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
         <v>168</v>
       </c>
@@ -10722,7 +11281,7 @@
         <v>31</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G169" s="7" t="b">
         <v>0</v>
@@ -10743,8 +11302,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="170" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R169" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
         <v>169</v>
       </c>
@@ -10779,8 +11341,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="171" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R170" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
         <v>170</v>
       </c>
@@ -10815,8 +11380,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="172" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R171" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
         <v>171</v>
       </c>
@@ -10851,8 +11419,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="173" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R172" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A173" s="7">
         <v>172</v>
       </c>
@@ -10887,8 +11458,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="174" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R173" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
         <v>173</v>
       </c>
@@ -10926,8 +11500,11 @@
         <f t="shared" si="4"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="175" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R174" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A175" s="7">
         <v>174</v>
       </c>
@@ -10962,8 +11539,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="176" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R175" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A176" s="7">
         <v>175</v>
       </c>
@@ -10998,8 +11578,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="177" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R176" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A177" s="7">
         <v>176</v>
       </c>
@@ -11034,8 +11617,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="178" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="R177" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" ht="119" x14ac:dyDescent="0.2">
       <c r="A178" s="7">
         <v>177</v>
       </c>
@@ -11073,8 +11659,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="179" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R178" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A179" s="7">
         <v>178</v>
       </c>
@@ -11109,8 +11698,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="180" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R179" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A180" s="7">
         <v>179</v>
       </c>
@@ -11145,8 +11737,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="181" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R180" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A181" s="7">
         <v>180</v>
       </c>
@@ -11181,8 +11776,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="182" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R181" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A182" s="7">
         <v>181</v>
       </c>
@@ -11220,8 +11818,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="183" spans="1:16" ht="153" x14ac:dyDescent="0.2">
+      <c r="R182" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" ht="153" x14ac:dyDescent="0.2">
       <c r="A183" s="7">
         <v>182</v>
       </c>
@@ -11259,8 +11860,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="184" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R183" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A184" s="7">
         <v>183</v>
       </c>
@@ -11298,8 +11902,11 @@
         <f t="shared" ref="P184:P186" si="7">IF(ISNUMBER(SEARCH("server", C184)), "Server", IF(ISNUMBER(SEARCH("Server", C184)), "Server", IF(ISNUMBER(SEARCH("client", C184)), "Client", IF(ISNUMBER(SEARCH("Client", C184)), "Client", ""))))</f>
         <v>Server</v>
       </c>
-    </row>
-    <row r="185" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R184" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A185" s="7">
         <v>184</v>
       </c>
@@ -11337,8 +11944,11 @@
         <f t="shared" si="7"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="186" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R185" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A186" s="7">
         <v>185</v>
       </c>
@@ -11376,8 +11986,11 @@
         <f t="shared" si="7"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="187" spans="1:16" ht="102" x14ac:dyDescent="0.2">
+      <c r="R186" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A187" s="7">
         <v>186</v>
       </c>
@@ -11412,8 +12025,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="188" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R187" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A188" s="7">
         <v>187</v>
       </c>
@@ -11448,8 +12064,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="189" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R188" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A189" s="7">
         <v>188</v>
       </c>
@@ -11484,8 +12103,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="190" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R189" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A190" s="7">
         <v>189</v>
       </c>
@@ -11520,8 +12142,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="191" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="R190" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
         <v>190</v>
       </c>
@@ -11556,8 +12181,11 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="192" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="R191" s="10" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A192" s="7">
         <v>191</v>
       </c>
@@ -11592,6 +12220,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R192" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="193" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A193" s="7">
@@ -11628,6 +12259,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R193" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="194" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A194" s="7">
@@ -11667,6 +12301,9 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
+      <c r="R194" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="195" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A195" s="7">
@@ -11703,6 +12340,9 @@
         <f t="shared" ref="P195:P258" si="8">IF(ISNUMBER(SEARCH("server", C195)), "Server", IF(ISNUMBER(SEARCH("Server", C195)), "Server", IF(ISNUMBER(SEARCH("client", C195)), "Client", IF(ISNUMBER(SEARCH("Client", C195)), "Client", ""))))</f>
         <v/>
       </c>
+      <c r="R195" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="196" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A196" s="7">
@@ -11742,6 +12382,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R196" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="197" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A197" s="7">
@@ -11778,6 +12421,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R197" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="198" spans="1:23" ht="136" x14ac:dyDescent="0.2">
       <c r="A198" s="7">
@@ -11817,6 +12463,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R198" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="199" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A199" s="7">
@@ -11853,6 +12502,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R199" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="200" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A200" s="7">
@@ -11889,6 +12541,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R200" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="201" spans="1:23" ht="85" x14ac:dyDescent="0.2">
       <c r="A201" s="7">
@@ -11931,6 +12586,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R201" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S201" s="16" t="s">
         <v>58</v>
       </c>
@@ -11982,6 +12640,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R202" s="10" t="s">
+        <v>486</v>
+      </c>
       <c r="S202" s="16" t="s">
         <v>80</v>
       </c>
@@ -12024,6 +12685,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R203" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="204" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A204" s="7">
@@ -12060,6 +12724,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R204" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="205" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A205" s="7">
@@ -12096,6 +12763,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R205" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="206" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A206" s="7">
@@ -12132,6 +12802,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R206" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="207" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A207" s="7">
@@ -12168,6 +12841,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R207" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="208" spans="1:23" ht="68" x14ac:dyDescent="0.2">
       <c r="A208" s="7">
@@ -12204,6 +12880,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R208" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="209" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A209" s="7">
@@ -12240,6 +12919,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R209" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="210" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A210" s="7">
@@ -12276,6 +12958,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R210" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="211" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A211" s="7">
@@ -12312,6 +12997,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R211" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="212" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A212" s="7">
@@ -12351,6 +13039,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R212" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="213" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A213" s="7">
@@ -12390,6 +13081,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R213" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="214" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A214" s="7">
@@ -12429,6 +13123,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R214" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="215" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A215" s="7">
@@ -12468,6 +13165,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R215" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="216" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A216" s="7">
@@ -12507,6 +13207,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R216" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="217" spans="1:22" ht="85" x14ac:dyDescent="0.2">
       <c r="A217" s="7">
@@ -12546,6 +13249,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R217" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="218" spans="1:22" ht="85" x14ac:dyDescent="0.2">
       <c r="A218" s="7">
@@ -12582,6 +13288,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R218" s="10" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="219" spans="1:22" ht="238" x14ac:dyDescent="0.2">
       <c r="A219" s="7">
@@ -12600,7 +13309,7 @@
         <v>31</v>
       </c>
       <c r="F219" s="29" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G219" s="7" t="b">
         <v>0</v>
@@ -12621,6 +13330,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R219" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="V219" s="16" t="s">
         <v>463</v>
       </c>
@@ -12696,6 +13408,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R221" s="10" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="222" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A222" s="7">
@@ -12705,7 +13420,7 @@
         <v>366</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D222" s="7" t="s">
         <v>37</v>
@@ -12735,6 +13450,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R222" s="10" t="s">
+        <v>484</v>
+      </c>
       <c r="S222" s="16" t="s">
         <v>80</v>
       </c>
@@ -12814,6 +13532,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R224" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="225" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A225" s="7">
@@ -12854,6 +13575,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R225" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="226" spans="1:22" ht="102" x14ac:dyDescent="0.2">
       <c r="A226" s="7">
@@ -12894,6 +13618,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R226" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="227" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A227" s="7">
@@ -12930,6 +13657,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R227" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="228" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A228" s="7">
@@ -12966,6 +13696,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R228" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="229" spans="1:22" ht="85" x14ac:dyDescent="0.2">
       <c r="A229" s="7">
@@ -13002,6 +13735,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R229" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="230" spans="1:22" ht="68" x14ac:dyDescent="0.2">
       <c r="A230" s="7">
@@ -13038,6 +13774,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R230" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="231" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A231" s="7">
@@ -13113,6 +13852,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R232" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="233" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A233" s="7">
@@ -13149,6 +13891,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R233" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="234" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A234" s="7">
@@ -13221,6 +13966,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R235" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="236" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A236" s="7">
@@ -13257,6 +14005,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R236" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="237" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A237" s="7">
@@ -13329,6 +14080,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R238" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="239" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A239" s="7">
@@ -13365,6 +14119,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R239" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="240" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A240" s="7">
@@ -13437,6 +14194,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R241" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="242" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="7">
@@ -13473,6 +14233,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R242" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="243" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A243" s="7">
@@ -13545,6 +14308,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R244" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="245" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A245" s="7">
@@ -13581,6 +14347,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R245" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="246" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A246" s="7">
@@ -13653,6 +14422,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R247" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="248" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A248" s="7">
@@ -13689,6 +14461,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R248" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="249" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A249" s="7">
@@ -13761,6 +14536,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R250" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="251" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A251" s="7">
@@ -13797,6 +14575,9 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="R251" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="252" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A252" s="7">
@@ -13833,6 +14614,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R252" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="253" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A253" s="7">
@@ -13872,6 +14656,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R253" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S253" s="16" t="s">
         <v>80</v>
       </c>
@@ -13947,6 +14734,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R255" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="256" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A256" s="7">
@@ -13986,6 +14776,9 @@
         <f t="shared" si="8"/>
         <v>Client</v>
       </c>
+      <c r="R256" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S256" s="16" t="s">
         <v>80</v>
       </c>
@@ -14061,6 +14854,9 @@
         <f t="shared" si="8"/>
         <v>Server</v>
       </c>
+      <c r="R258" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="259" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" s="7">
@@ -14100,6 +14896,9 @@
         <f t="shared" ref="P259:P272" si="10">IF(ISNUMBER(SEARCH("server", C259)), "Server", IF(ISNUMBER(SEARCH("Server", C259)), "Server", IF(ISNUMBER(SEARCH("client", C259)), "Client", IF(ISNUMBER(SEARCH("Client", C259)), "Client", ""))))</f>
         <v>Client</v>
       </c>
+      <c r="R259" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S259" s="16" t="s">
         <v>80</v>
       </c>
@@ -14175,6 +14974,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R261" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="262" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A262" s="7">
@@ -14214,6 +15016,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R262" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S262" s="16" t="s">
         <v>80</v>
       </c>
@@ -14289,6 +15094,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R264" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="265" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A265" s="7">
@@ -14328,6 +15136,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R265" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S265" s="16" t="s">
         <v>80</v>
       </c>
@@ -14403,6 +15214,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R267" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="268" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A268" s="7">
@@ -14442,6 +15256,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R268" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S268" s="16" t="s">
         <v>80</v>
       </c>
@@ -14517,6 +15334,9 @@
         <f t="shared" si="10"/>
         <v>Server</v>
       </c>
+      <c r="R270" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="271" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A271" s="7">
@@ -14556,6 +15376,9 @@
         <f t="shared" si="10"/>
         <v>Client</v>
       </c>
+      <c r="R271" s="10" t="s">
+        <v>488</v>
+      </c>
       <c r="S271" s="16" t="s">
         <v>80</v>
       </c>
@@ -14596,7 +15419,7 @@
         <v/>
       </c>
     </row>
-    <row r="273" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A273" s="7">
         <v>272</v>
       </c>
@@ -14631,8 +15454,11 @@
         <f>IF(ISNUMBER(SEARCH("server", C273)), "Server", IF(ISNUMBER(SEARCH("Server", C273)), "Server", IF(ISNUMBER(SEARCH("client", C273)), "Client", IF(ISNUMBER(SEARCH("Client", C273)), "Client", ""))))</f>
         <v>Server</v>
       </c>
-    </row>
-    <row r="274" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R273" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="274" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A274" s="7">
         <v>273</v>
       </c>
@@ -14667,8 +15493,11 @@
         <f t="shared" ref="P274:P298" si="12">IF(ISNUMBER(SEARCH("server", C274)), "Server", IF(ISNUMBER(SEARCH("Server", C274)), "Server", IF(ISNUMBER(SEARCH("client", C274)), "Client", IF(ISNUMBER(SEARCH("Client", C274)), "Client", ""))))</f>
         <v/>
       </c>
-    </row>
-    <row r="275" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R274" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="275" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A275" s="7">
         <v>274</v>
       </c>
@@ -14703,8 +15532,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="276" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R275" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="276" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A276" s="7">
         <v>275</v>
       </c>
@@ -14739,8 +15571,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="277" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R276" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="277" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A277" s="7">
         <v>276</v>
       </c>
@@ -14776,7 +15611,7 @@
         <v/>
       </c>
     </row>
-    <row r="278" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A278" s="7">
         <v>277</v>
       </c>
@@ -14811,8 +15646,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="279" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R278" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="279" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A279" s="7">
         <v>278</v>
       </c>
@@ -14847,8 +15685,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="280" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R279" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="280" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A280" s="7">
         <v>279</v>
       </c>
@@ -14884,7 +15725,7 @@
         <v/>
       </c>
     </row>
-    <row r="281" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A281" s="7">
         <v>280</v>
       </c>
@@ -14919,8 +15760,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="282" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R281" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="282" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A282" s="7">
         <v>281</v>
       </c>
@@ -14955,8 +15799,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="283" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R282" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="283" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A283" s="7">
         <v>282</v>
       </c>
@@ -14992,7 +15839,7 @@
         <v/>
       </c>
     </row>
-    <row r="284" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A284" s="7">
         <v>283</v>
       </c>
@@ -15027,8 +15874,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="285" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R284" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="285" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A285" s="7">
         <v>284</v>
       </c>
@@ -15063,8 +15913,11 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
-    </row>
-    <row r="286" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="R285" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="286" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A286" s="7">
         <v>285</v>
       </c>
@@ -15100,7 +15953,7 @@
         <v/>
       </c>
     </row>
-    <row r="287" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A287" s="7">
         <v>286</v>
       </c>
@@ -15135,8 +15988,11 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
-    </row>
-    <row r="288" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="R287" s="10" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="288" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A288" s="7">
         <v>287</v>
       </c>
@@ -15171,6 +16027,9 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
+      <c r="R288" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="289" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A289" s="7">
@@ -15243,6 +16102,9 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
+      <c r="R290" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="291" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A291" s="7">
@@ -15279,6 +16141,9 @@
         <f t="shared" si="12"/>
         <v>Client</v>
       </c>
+      <c r="R291" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="292" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A292" s="7">
@@ -15351,6 +16216,9 @@
         <f t="shared" si="12"/>
         <v>Server</v>
       </c>
+      <c r="R293" s="10" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="294" spans="1:31" ht="34" x14ac:dyDescent="0.2">
       <c r="A294" s="7">
@@ -15386,6 +16254,9 @@
       <c r="P294" s="10" t="str">
         <f t="shared" si="12"/>
         <v>Client</v>
+      </c>
+      <c r="R294" s="10" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="295" spans="1:31" ht="17" x14ac:dyDescent="0.2">
@@ -15466,7 +16337,9 @@
         <v>Server</v>
       </c>
       <c r="Q296" s="10"/>
-      <c r="R296" s="10"/>
+      <c r="R296" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="S296" s="16"/>
       <c r="T296" s="10"/>
       <c r="U296" s="10"/>
@@ -15475,7 +16348,7 @@
       </c>
       <c r="Y296" s="14"/>
     </row>
-    <row r="297" spans="1:31" s="58" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:31" s="58" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A297" s="7">
         <v>296</v>
       </c>
@@ -15517,7 +16390,9 @@
         <v/>
       </c>
       <c r="Q297" s="57"/>
-      <c r="R297" s="57"/>
+      <c r="R297" s="10" t="s">
+        <v>485</v>
+      </c>
       <c r="S297" s="54"/>
       <c r="T297" s="57"/>
       <c r="U297" s="57"/>
@@ -15566,7 +16441,9 @@
         <v>Server</v>
       </c>
       <c r="Q298" s="50"/>
-      <c r="R298" s="50"/>
+      <c r="R298" s="10" t="s">
+        <v>490</v>
+      </c>
       <c r="S298" s="47"/>
       <c r="T298" s="50"/>
       <c r="U298" s="50"/>
@@ -15588,6 +16465,9 @@
       <c r="E299" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R299" s="10" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="300" spans="1:31" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="7">
@@ -15605,6 +16485,9 @@
       <c r="E300" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R300" s="10" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="301" spans="1:31" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="7">
@@ -15622,6 +16505,9 @@
       <c r="E301" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R301" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="302" spans="1:31" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="7">
@@ -15639,6 +16525,9 @@
       <c r="E302" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R302" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="303" spans="1:31" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="7">
@@ -15656,6 +16545,9 @@
       <c r="E303" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R303" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="304" spans="1:31" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="7">
@@ -15673,6 +16565,9 @@
       <c r="E304" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R304" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="305" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="7">
@@ -15690,6 +16585,9 @@
       <c r="E305" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R305" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="306" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="7">
@@ -15707,6 +16605,9 @@
       <c r="E306" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R306" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="307" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="7">
@@ -15724,6 +16625,9 @@
       <c r="E307" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R307" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="308" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="7">
@@ -15741,6 +16645,9 @@
       <c r="E308" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R308" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="309" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="7">
@@ -15758,6 +16665,9 @@
       <c r="E309" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R309" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="310" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="7">
@@ -15775,6 +16685,9 @@
       <c r="E310" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R310" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="311" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="7">
@@ -15792,6 +16705,9 @@
       <c r="E311" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="R311" s="10" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="312" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="45">
@@ -15801,7 +16717,7 @@
         <v>71</v>
       </c>
       <c r="V312" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="313" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15812,7 +16728,7 @@
         <v>71</v>
       </c>
       <c r="V313" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="314" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15823,7 +16739,7 @@
         <v>71</v>
       </c>
       <c r="V314" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="315" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15834,7 +16750,7 @@
         <v>71</v>
       </c>
       <c r="V315" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="316" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15845,7 +16761,7 @@
         <v>71</v>
       </c>
       <c r="V316" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="317" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15856,7 +16772,7 @@
         <v>71</v>
       </c>
       <c r="V317" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="318" spans="1:22" ht="62" customHeight="1" x14ac:dyDescent="0.2">
@@ -15867,7 +16783,7 @@
         <v>71</v>
       </c>
       <c r="V318" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -15905,6 +16821,7 @@
     <hyperlink ref="B149" r:id="rId29" location="response---complete-status" xr:uid="{B0720E1E-4816-F842-82C8-C111E8C22B58}"/>
     <hyperlink ref="B229" r:id="rId30" location="bulkdataigcapabilitystatement" xr:uid="{4CF2CCA0-FA45-274E-B515-93FFD2130283}"/>
     <hyperlink ref="B228" r:id="rId31" location="bulkdataigcapabilitystatement" xr:uid="{5D27A2D1-DFBB-104F-ABC7-76F2A9211160}"/>
+    <hyperlink ref="B84" r:id="rId32" location="query-parameters" xr:uid="{32E0F273-4A07-D44B-AC1C-0A5D007653DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -15952,27 +16869,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C323F474-BE25-4449-9222-E1A46A1843B5}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="56.5" style="19" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="84.6640625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
-        <v>478</v>
-      </c>
-      <c r="B1" s="72"/>
+      <c r="A1" s="74" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
@@ -16051,6 +16968,14 @@
       </c>
       <c r="B13" s="19" t="s">
         <v>446</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="136" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>